<commit_message>
install required packages. minimal mods
</commit_message>
<xml_diff>
--- a/timings.xlsx
+++ b/timings.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0CA77B-4522-6142-A27E-47638B6030EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22320" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,22 +31,22 @@
     <t>Passcode</t>
   </si>
   <si>
-    <t>925 7400 2970</t>
-  </si>
-  <si>
-    <t>GE7ce7</t>
-  </si>
-  <si>
-    <t>225 7430 3970</t>
-  </si>
-  <si>
-    <t>Df3daf</t>
+    <t>838 0670 4556</t>
+  </si>
+  <si>
+    <t>863 8387 5679</t>
+  </si>
+  <si>
+    <t>doan training</t>
+  </si>
+  <si>
+    <t>practice partners</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -364,20 +365,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -388,26 +389,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0.73958333333333337</v>
+        <v>0.71527777777777779</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
+      <c r="C2">
+        <v>778530</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.67222222222222217</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>329714</v>
+      </c>
+      <c r="E3" t="s">
         <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>